<commit_message>
Updated the val_generator to work linearly through several songs
</commit_message>
<xml_diff>
--- a/SchulterReproduction/SchluterLog.xlsx
+++ b/SchulterReproduction/SchluterLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brendanoconnor/Desktop/APP/MXX-git2-/SchulterReproduction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16EAA162-F3BC-6F46-916C-2C38898B37F3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25FEC7A9-9C59-4F43-8E56-50C058142EAD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7280" yWindow="2680" windowWidth="28040" windowHeight="16520" xr2:uid="{0E031976-A5C9-AA40-B978-4DA5AD1A59FA}"/>
+    <workbookView xWindow="760" yWindow="460" windowWidth="28040" windowHeight="16500" xr2:uid="{0E031976-A5C9-AA40-B978-4DA5AD1A59FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -388,6 +388,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -397,14 +408,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="11" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -412,9 +415,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -734,7 +734,7 @@
   <dimension ref="A1:AH9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -749,152 +749,152 @@
     <col min="34" max="34" width="98.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:34" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="21"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="22"/>
       <c r="D1" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="11" t="s">
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12"/>
-      <c r="X1" s="12"/>
-      <c r="Y1" s="12"/>
-      <c r="Z1" s="12"/>
-      <c r="AA1" s="12"/>
-      <c r="AB1" s="12"/>
-      <c r="AC1" s="10" t="s">
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
+      <c r="T1" s="19"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="19"/>
+      <c r="W1" s="19"/>
+      <c r="X1" s="19"/>
+      <c r="Y1" s="19"/>
+      <c r="Z1" s="19"/>
+      <c r="AA1" s="19"/>
+      <c r="AB1" s="19"/>
+      <c r="AC1" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="AD1" s="10"/>
-      <c r="AE1" s="10"/>
-      <c r="AF1" s="10"/>
-      <c r="AG1" s="10"/>
-      <c r="AH1" s="22" t="s">
+      <c r="AD1" s="17"/>
+      <c r="AE1" s="17"/>
+      <c r="AF1" s="17"/>
+      <c r="AG1" s="17"/>
+      <c r="AH1" s="16" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:34" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:34" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="J2" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="K2" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="L2" s="15" t="s">
+      <c r="L2" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="15" t="s">
+      <c r="M2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="N2" s="15" t="s">
+      <c r="N2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="O2" s="15" t="s">
+      <c r="O2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="P2" s="15" t="s">
+      <c r="P2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="Q2" s="15" t="s">
+      <c r="Q2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="15" t="s">
+      <c r="R2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="15" t="s">
+      <c r="S2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="T2" s="15" t="s">
+      <c r="T2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="U2" s="15" t="s">
+      <c r="U2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="V2" s="15" t="s">
+      <c r="V2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="W2" s="15" t="s">
+      <c r="W2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="X2" s="15" t="s">
+      <c r="X2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="Y2" s="15" t="s">
+      <c r="Y2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="Z2" s="15" t="s">
+      <c r="Z2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="AA2" s="15" t="s">
+      <c r="AA2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="AB2" s="15" t="s">
+      <c r="AB2" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="AC2" s="15" t="s">
+      <c r="AC2" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="AD2" s="15" t="s">
+      <c r="AD2" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="AE2" s="15" t="s">
+      <c r="AE2" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AF2" s="15" t="s">
+      <c r="AF2" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="AG2" s="15" t="s">
+      <c r="AG2" s="12" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1357,7 +1357,7 @@
       <c r="W7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="X7" s="18">
+      <c r="X7" s="15">
         <v>1E-4</v>
       </c>
       <c r="Y7" s="1">

</xml_diff>